<commit_message>
Added Logo and Favicon
Added Logo and Favicon
</commit_message>
<xml_diff>
--- a/Web_Frontend/public/templates/student_upload_template.xlsx
+++ b/Web_Frontend/public/templates/student_upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayan\Documents\GitHub\EduSync\Web_Frontend\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6E6485-8F7D-4DCF-87CC-59FEB41CC4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A20B41B-A588-455F-AFCC-E2BB4948B744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8880" xr2:uid="{4C1367A3-E336-49FC-AEF4-109D15AB9821}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4C1367A3-E336-49FC-AEF4-109D15AB9821}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>fullName</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>div</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A491F3F1-523C-44E6-86E4-5B2EC61812BB}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,7 +459,7 @@
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -466,11 +472,17 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
     </row>
   </sheetData>

</xml_diff>